<commit_message>
added lambda function for ytrain
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="460" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="6880" yWindow="460" windowWidth="26720" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Company</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>601933</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>Average Return</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>Weighted return</t>
   </si>
 </sst>
 </file>
@@ -424,19 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="13.83203125" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,17 +477,32 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2">
+      <c r="Q1" s="2">
         <v>43878</v>
       </c>
-      <c r="P1" s="2">
+      <c r="R1" s="2">
         <v>43879</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S1" s="2">
+        <v>43880</v>
+      </c>
+      <c r="T1" s="2">
+        <v>43881</v>
+      </c>
+      <c r="U1" s="2">
+        <v>43882</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -495,32 +523,55 @@
         <f t="shared" ref="H2:H7" si="0">E2*F2-G2</f>
         <v>-5157.8999999999996</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2">
+        <f>G2/$N$2</f>
+        <v>0.13437000140677019</v>
+      </c>
+      <c r="K2">
+        <f>J2*I2</f>
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="L2">
-        <f>SUM(G2:G5,G7)</f>
-        <v>33310.6</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="N2">
+        <f>SUM(G2:G7)</f>
+        <v>38385.800000000003</v>
+      </c>
+      <c r="P2" s="1">
         <v>603993</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>600030</v>
       </c>
       <c r="B3" s="2">
         <v>43878</v>
       </c>
+      <c r="C3" s="2">
+        <v>43885</v>
+      </c>
       <c r="D3">
         <v>23.562999999999999</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
       </c>
       <c r="F3">
         <v>300</v>
@@ -531,27 +582,61 @@
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>-7068.9</v>
-      </c>
-      <c r="N3" s="1" t="s">
+        <v>431.10000000000036</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I4" si="2">H3/G3</f>
+        <v>6.0985443279718256E-2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J7" si="3">G3/$N$2</f>
+        <v>0.18415403612794312</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="4">J3*I3</f>
+        <v>1.1230715525011861E-2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3">
+        <f>SUM(H3:H7)</f>
+        <v>719.10000000000036</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O3">
-        <v>-1</v>
-      </c>
-      <c r="P3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>-1</v>
+      </c>
+      <c r="R3">
+        <v>-1</v>
+      </c>
+      <c r="S3">
+        <v>-1</v>
+      </c>
+      <c r="T3">
+        <v>-1</v>
+      </c>
+      <c r="U3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>43878</v>
       </c>
+      <c r="C4" s="2">
+        <v>43885</v>
+      </c>
       <c r="D4">
         <v>15.013</v>
+      </c>
+      <c r="E4">
+        <v>15.33</v>
       </c>
       <c r="F4">
         <v>400</v>
@@ -562,27 +647,61 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>-6005.2</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>126.80000000000018</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>2.1115033637514186E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.15644326808351003</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>3.3033048679459638E-3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4">
+        <f>SUM(K2:K7)</f>
+        <v>1.8733489988485327E-2</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>43878</v>
       </c>
+      <c r="C5" s="2">
+        <v>43881</v>
+      </c>
       <c r="D5">
         <v>57.36</v>
+      </c>
+      <c r="E5">
+        <v>62.55</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -593,19 +712,40 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>-5736</v>
-      </c>
-      <c r="N5" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="I5">
+        <f>H5/G5</f>
+        <v>9.0481171548117148E-2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>0.14943025806417998</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>1.3520624814384484E-2</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -636,17 +776,34 @@
         <f>H6/G6</f>
         <v>4.0983606557377407E-3</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>0.13221555887854361</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>5.4186704458419985E-4</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -655,6 +812,9 @@
       </c>
       <c r="D7">
         <v>15.571</v>
+      </c>
+      <c r="E7">
+        <v>14.94</v>
       </c>
       <c r="F7">
         <v>600</v>
@@ -665,203 +825,327 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>-9342.6</v>
-      </c>
-      <c r="N7" s="1" t="s">
+        <v>-378.60000000000036</v>
+      </c>
+      <c r="I7">
+        <f>H7/G7</f>
+        <v>-4.0524051120673081E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>0.24338687743905296</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>-9.8630222634411759E-3</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="N8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>-1</v>
+      </c>
+      <c r="S8">
+        <v>-1</v>
+      </c>
+      <c r="T8">
+        <v>-1</v>
+      </c>
+      <c r="U8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="N9" s="1" t="s">
+      <c r="J9">
+        <f>SUM(J2:J7)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O9">
-        <v>-1</v>
-      </c>
-      <c r="P9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <v>-1</v>
+      </c>
+      <c r="R9">
+        <v>-1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
+      <c r="U9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O10">
-        <v>-1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <v>-1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="N11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O11">
-        <v>-1</v>
-      </c>
-      <c r="P11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11">
+        <v>-1</v>
+      </c>
+      <c r="R11">
+        <v>-1</v>
+      </c>
+      <c r="S11">
+        <v>-1</v>
+      </c>
+      <c r="T11">
+        <v>-1</v>
+      </c>
+      <c r="U11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="N12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>-1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="N13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O13">
-        <v>-1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13">
+        <v>-1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="N14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>-1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="N15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O15">
-        <v>-1</v>
-      </c>
-      <c r="P15">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15">
+        <v>-1</v>
+      </c>
+      <c r="R15">
+        <v>-1</v>
+      </c>
+      <c r="S15">
+        <v>-1</v>
+      </c>
+      <c r="T15">
+        <v>-1</v>
+      </c>
+      <c r="U15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="N16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O16">
-        <v>-1</v>
-      </c>
-      <c r="P16">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16">
+        <v>-1</v>
+      </c>
+      <c r="R16">
+        <v>-1</v>
+      </c>
+      <c r="S16">
+        <v>-1</v>
+      </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
+      <c r="U16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="N17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>-1</v>
+      </c>
+      <c r="T17">
+        <v>-1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="N18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O18">
-        <v>-1</v>
-      </c>
-      <c r="P18">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <v>-1</v>
+      </c>
+      <c r="R18">
+        <v>-1</v>
+      </c>
+      <c r="S18">
+        <v>-1</v>
+      </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
+      <c r="U18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="N32" s="1"/>
     </row>

</xml_diff>